<commit_message>
fix: Wrong scale if NumberDataFormatter ends with "_)" - ExcelReader.cs update: Add test case for the fix - ExcelInTest.cs, A03.xlsx
</commit_message>
<xml_diff>
--- a/TestCase/xlsx/A03.xlsx
+++ b/TestCase/xlsx/A03.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C91F49-C33D-4050-B87A-9DD07D9F9EDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A03" sheetId="1" r:id="rId1"/>
@@ -73,56 +74,58 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="35">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="0.000%"/>
-    <numFmt numFmtId="165" formatCode="0.0000%"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.000_);[Red]\(&quot;$&quot;#,##0.000\)"/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.0_);[Red]\(&quot;$&quot;#,##0.0\)"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="m/d;@"/>
-    <numFmt numFmtId="170" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="171" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="172" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="173" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="174" formatCode="mmm\ d\,\ yyyy"/>
-    <numFmt numFmtId="175" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="176" formatCode="#,##0.00\ [$₽-419]"/>
-    <numFmt numFmtId="177" formatCode="[$¥-804]#,##0.00"/>
-    <numFmt numFmtId="178" formatCode="[$¥-411]#,##0.00"/>
-    <numFmt numFmtId="179" formatCode="[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="180" formatCode="[$JPY]\ #,##0.00"/>
-    <numFmt numFmtId="181" formatCode="#,##0.00\ [$€-407]"/>
-    <numFmt numFmtId="182" formatCode="[$₱-3409]#,##0.00"/>
-    <numFmt numFmtId="183" formatCode="[$USD]\ #,##0.00"/>
-    <numFmt numFmtId="184" formatCode="&quot;$&quot;#,##0.0000"/>
-    <numFmt numFmtId="185" formatCode="#,##0.0000\ [$₽-419]"/>
-    <numFmt numFmtId="186" formatCode="[$¥-804]#,##0.0000"/>
-    <numFmt numFmtId="187" formatCode="[$¥-411]#,##0.0000"/>
-    <numFmt numFmtId="188" formatCode="[$€-2]\ #,##0.0000"/>
-    <numFmt numFmtId="189" formatCode="[$JPY]\ #,##0.0000"/>
-    <numFmt numFmtId="190" formatCode="#,##0.0000\ [$€-407]"/>
-    <numFmt numFmtId="191" formatCode="[$₱-3409]#,##0.0000"/>
-    <numFmt numFmtId="192" formatCode="[$USD]\ #,##0.0000"/>
-    <numFmt numFmtId="193" formatCode="0.00;[Red]0.00"/>
-    <numFmt numFmtId="194" formatCode="0.00_);\(0.00\)"/>
-    <numFmt numFmtId="195" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="198" formatCode="#,##0_);&quot;▲ &quot;#,##0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="37">
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="178" formatCode="0.000%"/>
+    <numFmt numFmtId="179" formatCode="0.0000%"/>
+    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,##0.000_);[Red]\(&quot;$&quot;#,##0.000\)"/>
+    <numFmt numFmtId="181" formatCode="&quot;$&quot;#,##0.0_);[Red]\(&quot;$&quot;#,##0.0\)"/>
+    <numFmt numFmtId="182" formatCode="0.0%"/>
+    <numFmt numFmtId="183" formatCode="m/d;@"/>
+    <numFmt numFmtId="184" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="185" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="186" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="187" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="188" formatCode="mmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="189" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="190" formatCode="#,##0.00\ [$₽-419]"/>
+    <numFmt numFmtId="191" formatCode="[$¥-804]#,##0.00"/>
+    <numFmt numFmtId="192" formatCode="[$¥-411]#,##0.00"/>
+    <numFmt numFmtId="193" formatCode="[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="194" formatCode="[$JPY]\ #,##0.00"/>
+    <numFmt numFmtId="195" formatCode="#,##0.00\ [$€-407]"/>
+    <numFmt numFmtId="196" formatCode="[$₱-3409]#,##0.00"/>
+    <numFmt numFmtId="197" formatCode="[$USD]\ #,##0.00"/>
+    <numFmt numFmtId="198" formatCode="&quot;$&quot;#,##0.0000"/>
+    <numFmt numFmtId="199" formatCode="#,##0.0000\ [$₽-419]"/>
+    <numFmt numFmtId="200" formatCode="[$¥-804]#,##0.0000"/>
+    <numFmt numFmtId="201" formatCode="[$¥-411]#,##0.0000"/>
+    <numFmt numFmtId="202" formatCode="[$€-2]\ #,##0.0000"/>
+    <numFmt numFmtId="203" formatCode="[$JPY]\ #,##0.0000"/>
+    <numFmt numFmtId="204" formatCode="#,##0.0000\ [$€-407]"/>
+    <numFmt numFmtId="205" formatCode="[$₱-3409]#,##0.0000"/>
+    <numFmt numFmtId="206" formatCode="[$USD]\ #,##0.0000"/>
+    <numFmt numFmtId="207" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="208" formatCode="0.00_);\(0.00\)"/>
+    <numFmt numFmtId="209" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="210" formatCode="#,##0_);&quot;▲ &quot;#,##0"/>
+    <numFmt numFmtId="211" formatCode="[$CNY]\ #,##0.00_);\([$CNY]\ #,##0.00\)"/>
+    <numFmt numFmtId="212" formatCode="[$CNY]\ #,##0.0000_);\([$CNY]\ #,##0.0000\)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -130,7 +133,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -138,13 +141,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -152,7 +155,7 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -160,22 +163,29 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -205,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -244,21 +254,21 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -266,20 +276,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -287,10 +283,26 @@
     <xf numFmtId="193" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="194" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="196" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="197" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="198" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="199" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="200" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="201" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="202" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="203" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="204" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="205" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="206" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="207" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="208" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="209" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="210" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="211" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="212" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -306,7 +318,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -381,6 +393,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -416,6 +445,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -591,25 +637,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="1" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,7 +667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -631,7 +678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="22.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -642,7 +689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
@@ -654,7 +701,7 @@
       </c>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
@@ -665,7 +712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>8</v>
       </c>
@@ -676,7 +723,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -705,7 +752,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="25">
         <v>1</v>
       </c>
@@ -734,7 +781,7 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.1</v>
       </c>
@@ -763,7 +810,7 @@
         <v>0.123456789</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>0</v>
       </c>
@@ -792,7 +839,7 @@
         <v>12.34</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
         <v>1E-3</v>
       </c>
@@ -821,7 +868,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>41974</v>
       </c>
@@ -844,7 +891,7 @@
         <v>41980</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
         <v>16</v>
       </c>
@@ -852,7 +899,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
         <v>1</v>
       </c>
@@ -880,8 +927,11 @@
       <c r="I15" s="46">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="60">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="38">
         <v>1234</v>
       </c>
@@ -909,8 +959,11 @@
       <c r="I16" s="46">
         <v>1234</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="60">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="38">
         <v>-1.234</v>
       </c>
@@ -938,8 +991,11 @@
       <c r="I17" s="46">
         <v>-1.234</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="60">
+        <v>-1.234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="47">
         <v>-1.234</v>
       </c>
@@ -967,13 +1023,16 @@
       <c r="I18" s="55">
         <v>-1.234</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J18" s="61">
+        <v>-1.234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-10</v>
       </c>
@@ -991,6 +1050,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>